<commit_message>
Update to accommodate the new folder structure
Tested on SimPathsStart.
</commit_message>
<xml_diff>
--- a/input/EL/EUROMODpolicySchedule.xlsx
+++ b/input/EL/EUROMODpolicySchedule.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="77">
   <si>
     <t>Filename</t>
   </si>
@@ -634,7 +634,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -648,13 +648,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -662,13 +662,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -676,13 +676,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -690,13 +690,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -704,13 +704,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -718,13 +718,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -732,13 +732,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -746,13 +746,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -774,13 +774,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -788,13 +788,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -802,13 +802,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -816,13 +816,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
@@ -914,13 +914,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -956,13 +956,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -1096,13 +1096,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -1194,13 +1194,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
@@ -1236,13 +1236,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -1320,13 +1320,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
         <v>13</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
         <v>13</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>13</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
         <v>13</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>

</xml_diff>